<commit_message>
started writing the trading system class implement getCart and getBasket
</commit_message>
<xml_diff>
--- a/Docs/Use Cases and Acceptance Tests.xlsx
+++ b/Docs/Use Cases and Acceptance Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lidor\BGU 2021 Semester B\סדנה\version 0\תרחישי שימוש\נעה ועמרי\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97254\Desktop\TradingSystem\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC096E1-6692-4858-A028-7EF45D17BA1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC1F688-D4D1-4A16-B8ED-360B96790020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usecase1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
         <b/>
         <sz val="14"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -71,7 +71,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -461,7 +461,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -512,7 +512,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -528,7 +528,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -544,7 +544,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -560,7 +560,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -577,7 +577,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -587,7 +587,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -597,7 +597,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -882,7 +882,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -988,7 +988,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -998,7 +998,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1558,7 +1558,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1566,7 +1566,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1574,27 +1574,27 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1602,7 +1602,7 @@
       <b/>
       <sz val="26"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1755,28 +1755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1786,6 +1765,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2070,46 +2070,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A12" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.21875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.4140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.25" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.75" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.75" style="5" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="40.5546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="42.77734375" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="8.77734375" style="3"/>
+    <col min="7" max="7" width="40.58203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="42.75" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.75" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -2137,7 +2137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="98" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2.1</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="98" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>2.4</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2.5</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2.6</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>2.7</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>62</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>66</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="154" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>63</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="98" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>64</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="168" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>2.9</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>3.1</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="98" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>3.2</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="70" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>3.7</v>
       </c>
@@ -2701,27 +2701,27 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.58203125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.75" customWidth="1"/>
+    <col min="4" max="4" width="21.4140625" customWidth="1"/>
     <col min="5" max="5" width="29.6640625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -2740,7 +2740,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2.1</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2.1</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2.4</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2.4</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>2.5</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>2.5</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="70" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>2.6</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>2.6</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>2.6</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>2.6</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="56" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>2.7</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="56" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>2.7</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>66</v>
       </c>
@@ -3131,14 +3131,14 @@
         <v>286</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="17" t="s">
         <v>284</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -3148,7 +3148,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>64</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="56" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>64</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>65</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="56" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>64</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="70" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="70" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>2.9</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="56" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>2.9</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>94</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>94</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>3.1</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>3.1</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="56" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>3.2</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="56" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>3.2</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>3.7</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>3.7</v>
       </c>
@@ -3438,41 +3438,41 @@
       <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="37.77734375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="25.77734375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="6.4140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="18.75" style="11" customWidth="1"/>
+    <col min="3" max="3" width="37.75" style="11" customWidth="1"/>
+    <col min="4" max="4" width="29.75" style="11" customWidth="1"/>
+    <col min="5" max="5" width="25.75" style="12" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="27.4140625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="30.08203125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -3500,7 +3500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>4.0999999999999996</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>230</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>231</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4.3</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>4.5</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>4.5999999999999996</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>4.7</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>4.9000000000000004</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>4.1100000000000003</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>5.0999999999999996</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="98" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>6.4</v>
       </c>
@@ -3804,27 +3804,27 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.08203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="38.21875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="38.25" style="3" customWidth="1"/>
+    <col min="5" max="5" width="40.9140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
@@ -3843,14 +3843,14 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="25" t="s">
         <v>325</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -3864,8 +3864,8 @@
       <c r="A4" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="1" t="s">
         <v>328</v>
       </c>
@@ -3873,12 +3873,12 @@
         <v>329</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="1" t="s">
         <v>330</v>
       </c>
@@ -3886,12 +3886,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="1" t="s">
         <v>332</v>
       </c>
@@ -3899,12 +3899,12 @@
         <v>333</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="25" t="s">
         <v>334</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -3914,12 +3914,12 @@
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="1" t="s">
         <v>337</v>
       </c>
@@ -3931,10 +3931,10 @@
       <c r="A9" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="25" t="s">
         <v>339</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -3944,12 +3944,12 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="1" t="s">
         <v>342</v>
       </c>
@@ -3957,12 +3957,12 @@
         <v>343</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="27"/>
+      <c r="C11" s="25" t="s">
         <v>344</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -3972,12 +3972,12 @@
         <v>346</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="1" t="s">
         <v>347</v>
       </c>
@@ -3989,10 +3989,10 @@
       <c r="A13" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="25" t="s">
         <v>349</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -4002,12 +4002,12 @@
         <v>350</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="1" t="s">
         <v>342</v>
       </c>
@@ -4015,12 +4015,12 @@
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="22" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="25" t="s">
         <v>351</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -4030,12 +4030,12 @@
         <v>346</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="1" t="s">
         <v>353</v>
       </c>
@@ -4047,10 +4047,10 @@
       <c r="A17" s="7">
         <v>4.3</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="25" t="s">
         <v>159</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -4060,12 +4060,12 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>4.3</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="1" t="s">
         <v>357</v>
       </c>
@@ -4077,10 +4077,10 @@
       <c r="A19" s="7">
         <v>4.5</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="25" t="s">
         <v>166</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -4094,8 +4094,8 @@
       <c r="A20" s="7">
         <v>4.5</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="1" t="s">
         <v>361</v>
       </c>
@@ -4107,8 +4107,8 @@
       <c r="A21" s="7">
         <v>4.5</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="1" t="s">
         <v>362</v>
       </c>
@@ -4120,8 +4120,8 @@
       <c r="A22" s="7">
         <v>4.5</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="1" t="s">
         <v>363</v>
       </c>
@@ -4133,8 +4133,8 @@
       <c r="A23" s="7">
         <v>4.5</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="1" t="s">
         <v>365</v>
       </c>
@@ -4142,14 +4142,14 @@
         <v>366</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="25" t="s">
         <v>367</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -4159,12 +4159,12 @@
         <v>369</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="1" t="s">
         <v>370</v>
       </c>
@@ -4172,12 +4172,12 @@
         <v>371</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="1" t="s">
         <v>372</v>
       </c>
@@ -4185,12 +4185,12 @@
         <v>373</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="1" t="s">
         <v>374</v>
       </c>
@@ -4198,14 +4198,14 @@
         <v>375</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>4.7</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="25" t="s">
         <v>376</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -4215,12 +4215,12 @@
         <v>378</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>4.7</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="1" t="s">
         <v>379</v>
       </c>
@@ -4228,14 +4228,14 @@
         <v>380</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="25" t="s">
         <v>185</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -4249,8 +4249,8 @@
       <c r="A31" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="1" t="s">
         <v>383</v>
       </c>
@@ -4258,14 +4258,14 @@
         <v>384</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>4.1100000000000003</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="25" t="s">
         <v>385</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -4279,8 +4279,8 @@
       <c r="A33" s="7">
         <v>4.1100000000000003</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="1" t="s">
         <v>383</v>
       </c>
@@ -4288,14 +4288,14 @@
         <v>384</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>6.4</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="25" t="s">
         <v>386</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -4309,8 +4309,8 @@
       <c r="A35" s="7">
         <v>6.4</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="1" t="s">
         <v>389</v>
       </c>
@@ -4318,12 +4318,12 @@
         <v>390</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>6.4</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="22" t="s">
+      <c r="B36" s="27"/>
+      <c r="C36" s="25" t="s">
         <v>391</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -4337,8 +4337,8 @@
       <c r="A37" s="7">
         <v>6.4</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="1" t="s">
         <v>394</v>
       </c>
@@ -4346,12 +4346,12 @@
         <v>390</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>6.4</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="22" t="s">
+      <c r="B38" s="27"/>
+      <c r="C38" s="25" t="s">
         <v>395</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -4365,8 +4365,8 @@
       <c r="A39" s="7">
         <v>6.4</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="1" t="s">
         <v>398</v>
       </c>
@@ -4378,8 +4378,8 @@
       <c r="A40" s="7">
         <v>6.4</v>
       </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
       <c r="D40" s="1" t="s">
         <v>399</v>
       </c>
@@ -4389,23 +4389,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="C19:C23"/>
     <mergeCell ref="A1:H1"/>
@@ -4415,6 +4398,23 @@
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4428,41 +4428,41 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="36.21875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.4140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.4140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="36.25" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.75" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.75" style="5" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="27.4140625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="30.08203125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -4490,33 +4490,33 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="25">
+    <row r="4" spans="1:8" ht="112" x14ac:dyDescent="0.3">
+      <c r="A4" s="18">
         <v>7</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="19" t="s">
         <v>204</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="20" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>8</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>232</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>233</v>
       </c>
@@ -4612,27 +4612,27 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.4140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.75" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.4140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="36.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -4651,7 +4651,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>7</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>7</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>8</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>232</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>232</v>
       </c>
@@ -4736,7 +4736,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>233</v>
       </c>

</xml_diff>

<commit_message>
changes to the TradingSystemService after teem meeting.
</commit_message>
<xml_diff>
--- a/Docs/Use Cases and Acceptance Tests.xlsx
+++ b/Docs/Use Cases and Acceptance Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97254\Desktop\TradingSystem\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC1F688-D4D1-4A16-B8ED-360B96790020}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131C053A-F983-443C-B1BB-97015534551F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usecase1" sheetId="1" r:id="rId1"/>
@@ -366,9 +366,6 @@
   </si>
   <si>
     <t>2.9.1</t>
-  </si>
-  <si>
-    <t>רכישת מוצרים לפי מדיניות עבור סל קניות ספציפי</t>
   </si>
   <si>
     <t>המערכת תבצע את רכישת המשתמש בהתאם למדיניות עבור סל הקניות</t>
@@ -1548,6 +1545,9 @@
   </si>
   <si>
     <t>עגלת הקניות עם אותו מזהה אינה השתנתה והוחזרה הודעת שגיאה.</t>
+  </si>
+  <si>
+    <t>חישוב מוצרים לפי מדיניות עבור סל קניות ספציפי</t>
   </si>
 </sst>
 </file>
@@ -1782,10 +1782,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2070,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A12" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView rightToLeft="1" topLeftCell="A21" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -2151,13 +2151,13 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>14</v>
@@ -2177,13 +2177,13 @@
         <v>12</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
@@ -2203,7 +2203,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>21</v>
@@ -2223,19 +2223,19 @@
         <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>26</v>
@@ -2249,7 +2249,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -2261,10 +2261,10 @@
         <v>29</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="56" x14ac:dyDescent="0.3">
@@ -2278,10 +2278,10 @@
         <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>32</v>
@@ -2304,7 +2304,7 @@
         <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>36</v>
@@ -2330,10 +2330,10 @@
         <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>42</v>
@@ -2350,16 +2350,16 @@
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>54</v>
@@ -2382,10 +2382,10 @@
         <v>53</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>55</v>
@@ -2394,7 +2394,7 @@
         <v>59</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="84" x14ac:dyDescent="0.3">
@@ -2408,7 +2408,7 @@
         <v>68</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>57</v>
@@ -2420,7 +2420,7 @@
         <v>60</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="42" x14ac:dyDescent="0.3">
@@ -2434,10 +2434,10 @@
         <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>70</v>
@@ -2460,13 +2460,13 @@
         <v>72</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>73</v>
@@ -2486,7 +2486,7 @@
         <v>77</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>78</v>
@@ -2512,7 +2512,7 @@
         <v>83</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>84</v>
@@ -2538,7 +2538,7 @@
         <v>88</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>84</v>
@@ -2564,19 +2564,19 @@
         <v>93</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
@@ -2584,25 +2584,25 @@
         <v>94</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="56" x14ac:dyDescent="0.3">
@@ -2610,25 +2610,25 @@
         <v>3.1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="98" x14ac:dyDescent="0.3">
@@ -2636,25 +2636,25 @@
         <v>3.2</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="G23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="70" x14ac:dyDescent="0.3">
@@ -2662,25 +2662,25 @@
         <v>3.7</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2713,7 +2713,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -2728,16 +2728,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>237</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="42" x14ac:dyDescent="0.3">
@@ -2745,16 +2745,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -2762,16 +2762,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -2785,10 +2785,10 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
@@ -2802,10 +2802,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -2819,10 +2819,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -2836,10 +2836,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="42" x14ac:dyDescent="0.3">
@@ -2850,13 +2850,13 @@
         <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="56" x14ac:dyDescent="0.3">
@@ -2867,13 +2867,13 @@
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.3">
@@ -2884,13 +2884,13 @@
         <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.3">
@@ -2901,13 +2901,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -2918,13 +2918,13 @@
         <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -2935,13 +2935,13 @@
         <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -2952,13 +2952,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -2969,13 +2969,13 @@
         <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="70" x14ac:dyDescent="0.3">
@@ -2986,13 +2986,13 @@
         <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3003,13 +3003,13 @@
         <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3020,13 +3020,13 @@
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -3037,13 +3037,13 @@
         <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="56" x14ac:dyDescent="0.3">
@@ -3054,13 +3054,13 @@
         <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="56" x14ac:dyDescent="0.3">
@@ -3071,13 +3071,13 @@
         <v>56</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -3088,13 +3088,13 @@
         <v>61</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -3105,13 +3105,13 @@
         <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3122,13 +3122,13 @@
         <v>61</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3139,13 +3139,13 @@
         <v>61</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3156,13 +3156,13 @@
         <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="56" x14ac:dyDescent="0.3">
@@ -3173,13 +3173,13 @@
         <v>61</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3190,13 +3190,13 @@
         <v>61</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="56" x14ac:dyDescent="0.3">
@@ -3207,13 +3207,13 @@
         <v>61</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3224,13 +3224,13 @@
         <v>61</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="70" x14ac:dyDescent="0.3">
@@ -3241,13 +3241,13 @@
         <v>61</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="70" x14ac:dyDescent="0.3">
@@ -3258,13 +3258,13 @@
         <v>92</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="56" x14ac:dyDescent="0.3">
@@ -3275,13 +3275,13 @@
         <v>92</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3292,13 +3292,13 @@
         <v>92</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3309,13 +3309,13 @@
         <v>92</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -3323,16 +3323,16 @@
         <v>3.1</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3340,16 +3340,16 @@
         <v>3.1</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="56" x14ac:dyDescent="0.3">
@@ -3357,16 +3357,16 @@
         <v>3.2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="56" x14ac:dyDescent="0.3">
@@ -3374,16 +3374,16 @@
         <v>3.2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3391,16 +3391,16 @@
         <v>3.7</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -3408,16 +3408,16 @@
         <v>3.7</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -3505,77 +3505,77 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>151</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="126" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="84" x14ac:dyDescent="0.3">
@@ -3583,25 +3583,25 @@
         <v>4.3</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="126" x14ac:dyDescent="0.3">
@@ -3609,25 +3609,25 @@
         <v>4.5</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="84" x14ac:dyDescent="0.3">
@@ -3635,25 +3635,25 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="84" x14ac:dyDescent="0.3">
@@ -3661,25 +3661,25 @@
         <v>4.7</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="56" x14ac:dyDescent="0.3">
@@ -3687,25 +3687,25 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>187</v>
-      </c>
       <c r="H11" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.3">
@@ -3713,25 +3713,25 @@
         <v>4.1100000000000003</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>190</v>
-      </c>
       <c r="H12" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="56" x14ac:dyDescent="0.3">
@@ -3739,25 +3739,25 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="98" x14ac:dyDescent="0.3">
@@ -3765,25 +3765,25 @@
         <v>6.4</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>201</v>
-      </c>
       <c r="H14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3816,7 +3816,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -3831,16 +3831,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -3848,199 +3848,199 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>328</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>340</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="26"/>
+        <v>229</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="B11" s="27"/>
+        <v>229</v>
+      </c>
+      <c r="B11" s="26"/>
       <c r="C11" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+        <v>229</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="26"/>
+        <v>230</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B15" s="27"/>
+        <v>230</v>
+      </c>
+      <c r="B15" s="26"/>
       <c r="C15" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
+        <v>230</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -4048,29 +4048,29 @@
         <v>4.3</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>4.3</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -4078,68 +4078,68 @@
         <v>4.5</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>4.5</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>4.5</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>4.5</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>4.5</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.3">
@@ -4147,55 +4147,55 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="42" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="28" x14ac:dyDescent="0.3">
@@ -4203,29 +4203,29 @@
         <v>4.7</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C28" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>4.7</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>379</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4233,29 +4233,29 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4263,29 +4263,29 @@
         <v>4.1100000000000003</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>4.1100000000000003</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>383</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4293,102 +4293,114 @@
         <v>6.4</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C34" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>6.4</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="28" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>6.4</v>
       </c>
-      <c r="B36" s="27"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>6.4</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>6.4</v>
       </c>
-      <c r="B38" s="27"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>6.4</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>6.4</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>400</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="C19:C23"/>
     <mergeCell ref="A1:H1"/>
@@ -4403,18 +4415,6 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4424,7 +4424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071701CE-A324-4452-B698-F2E194D1AE4B}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="71" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -4454,7 +4454,7 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -4495,25 +4495,25 @@
         <v>7</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="E4" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="F4" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="G4" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="H4" s="20" t="s">
         <v>209</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="126" x14ac:dyDescent="0.3">
@@ -4521,77 +4521,77 @@
         <v>8</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="H5" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B6" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="H6" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="H7" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -4624,7 +4624,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -4639,16 +4639,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -4656,16 +4656,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -4673,16 +4673,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
@@ -4690,67 +4690,67 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="D8" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added use cases for V2
</commit_message>
<xml_diff>
--- a/Docs/Use Cases and Acceptance Tests.xlsx
+++ b/Docs/Use Cases and Acceptance Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97254\Desktop\TradingSystem\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lidor\BGU 2021 Semester B\סדנה\version 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131C053A-F983-443C-B1BB-97015534551F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58D242D5-5961-4F70-B02C-5DB76B5500FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34635" yWindow="6045" windowWidth="13830" windowHeight="7170" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usecase1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="444">
   <si>
     <t>שם תרחיש השימוש</t>
   </si>
@@ -61,7 +61,7 @@
         <b/>
         <sz val="14"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -71,7 +71,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -458,7 +458,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -509,7 +509,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -525,7 +525,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -541,7 +541,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -557,7 +557,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -574,7 +574,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -584,7 +584,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -594,7 +594,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -879,7 +879,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -985,7 +985,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -995,7 +995,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1548,6 +1548,96 @@
   </si>
   <si>
     <t>חישוב מוצרים לפי מדיניות עבור סל קניות ספציפי</t>
+  </si>
+  <si>
+    <t>הסרת מינוי של בעל חנות</t>
+  </si>
+  <si>
+    <t>בעל-חנות רשאי להסיר מינוי של בעל-חנות שמונה על ידו בעבר. הסרת מינוי של בעל חנות גוררת הסרת כל המינויים של בעלי ומנהלי החנות שמונו על ידו</t>
+  </si>
+  <si>
+    <t>מוכרים בעלי חנות (אופציונאלי: מנהלי חנות)</t>
+  </si>
+  <si>
+    <t>1. בעל החנות logged in למנוי שלו
+2. החנות בבעלות המנוי
+3. המנוי המוסר מונה ע"י המסיר</t>
+  </si>
+  <si>
+    <t>1. המנוי שהוסר ללא הרשאות בחנות.
+2. בעלי תפקידים שמונו ע"י המנוי המוסר - ללא הרשאות בחנות</t>
+  </si>
+  <si>
+    <t>1. בעל חנות בוחר להסיר מינוי של בעלים שהוא מינה
+2. בעל החנות שנבחר וכן מי שמונה על ידו, מוסרים מתפקידיהם בחנות</t>
+  </si>
+  <si>
+    <t>2'. ניסיון להסיר מישהו שלא מונה ע"י המסיר יגרום לשגיאה.</t>
+  </si>
+  <si>
+    <t>התראות זמן אמת</t>
+  </si>
+  <si>
+    <t>בעלי חנות, קונה</t>
+  </si>
+  <si>
+    <t>9.1.1</t>
+  </si>
+  <si>
+    <t>9.1.2</t>
+  </si>
+  <si>
+    <t>בעלי חנות צריכים לקבל התראת זמן-אמת כאשר לקוח קונה מוצר מחנותם</t>
+  </si>
+  <si>
+    <t>בעלי חנות צריכים לקבל התראת זמן-אמת כאשר
+חנותם נסגרת או נפתחת מחדש</t>
+  </si>
+  <si>
+    <t>בעלי חנות צריכים לקבל התראת זמן-אמת כאשר המינוי שלהם מוסר</t>
+  </si>
+  <si>
+    <t>9.1.3</t>
+  </si>
+  <si>
+    <t>התקבלה התראה אצל בעל החנות</t>
+  </si>
+  <si>
+    <t>משתמש קונה מבצע רכישה בחנות. בעל החנות מקבל התראה על הרכישה</t>
+  </si>
+  <si>
+    <t>בעל החנות אינו מחובר למערכת. ההתראה תושהה ותוצג לו כשיתחבר</t>
+  </si>
+  <si>
+    <t>בעלי חנות</t>
+  </si>
+  <si>
+    <t>בעלי חנות, מנהל מערכת</t>
+  </si>
+  <si>
+    <t>בעלי החנות מקבלים התראה על פתיחת/סגירת החנות</t>
+  </si>
+  <si>
+    <t>מנהל מערכת סוגר/פותח מחדש חנות. בעלי החנות מקבלים התראה על הפעולה</t>
+  </si>
+  <si>
+    <t>בעלים או מנהל מערכת סוגר או פותח חנות מחדש</t>
+  </si>
+  <si>
+    <t>משתמש קונה מוצר מהחנות.
+בעל החנות מחובר למערכת</t>
+  </si>
+  <si>
+    <t>בעלים מסיר מינוי של בעל/מנהל חנות</t>
+  </si>
+  <si>
+    <t>המנוי שהוסר מינויו מקבל התראה</t>
+  </si>
+  <si>
+    <t>בעל חנות מסיר מינוי של בעלים/מנהל חנות. המנוי שהוסר מינויו מקבל התראה</t>
+  </si>
+  <si>
+    <t>המנוי אינו מחובר למערכת. ההתראה תושהה ותוצג לו כשיתחבר</t>
   </si>
 </sst>
 </file>
@@ -1558,7 +1648,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1566,7 +1656,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1574,27 +1664,27 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1602,7 +1692,7 @@
       <b/>
       <sz val="26"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1782,10 +1872,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2074,17 +2164,17 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.4140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.25" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.75" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.75" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" style="5" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="40.58203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="42.75" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="8.75" style="3"/>
+    <col min="7" max="7" width="40.5546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="42.77734375" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
@@ -2137,7 +2227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="98" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -2163,7 +2253,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2.1</v>
       </c>
@@ -2189,7 +2279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2215,7 +2305,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -2241,7 +2331,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="98" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>2.4</v>
       </c>
@@ -2267,7 +2357,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2.5</v>
       </c>
@@ -2293,7 +2383,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
@@ -2319,7 +2409,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2.6</v>
       </c>
@@ -2345,7 +2435,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
@@ -2371,7 +2461,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
@@ -2397,7 +2487,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>2.7</v>
       </c>
@@ -2423,7 +2513,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>62</v>
       </c>
@@ -2449,7 +2539,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>66</v>
       </c>
@@ -2475,7 +2565,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="154" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>63</v>
       </c>
@@ -2501,7 +2591,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="98" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>64</v>
       </c>
@@ -2553,7 +2643,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="168" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>2.9</v>
       </c>
@@ -2605,7 +2695,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>3.1</v>
       </c>
@@ -2631,7 +2721,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="98" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>3.2</v>
       </c>
@@ -2657,7 +2747,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="70" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>3.7</v>
       </c>
@@ -2701,12 +2791,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.58203125" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="23.75" customWidth="1"/>
-    <col min="4" max="4" width="21.4140625" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="29.6640625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
@@ -2740,7 +2830,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -2757,7 +2847,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -2774,7 +2864,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2.1</v>
       </c>
@@ -2791,7 +2881,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2.1</v>
       </c>
@@ -2808,7 +2898,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2825,7 +2915,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2842,7 +2932,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -2859,7 +2949,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -2876,7 +2966,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2.4</v>
       </c>
@@ -2893,7 +2983,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2.4</v>
       </c>
@@ -2910,7 +3000,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>2.5</v>
       </c>
@@ -2927,7 +3017,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>2.5</v>
       </c>
@@ -2944,7 +3034,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>38</v>
       </c>
@@ -2961,7 +3051,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
@@ -2978,7 +3068,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="70" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>2.6</v>
       </c>
@@ -2995,7 +3085,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>2.6</v>
       </c>
@@ -3012,7 +3102,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>2.6</v>
       </c>
@@ -3029,7 +3119,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>2.6</v>
       </c>
@@ -3046,7 +3136,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>2.7</v>
       </c>
@@ -3063,7 +3153,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>2.7</v>
       </c>
@@ -3080,7 +3170,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
@@ -3097,7 +3187,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
@@ -3114,7 +3204,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>66</v>
       </c>
@@ -3131,7 +3221,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>66</v>
       </c>
@@ -3148,7 +3238,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>64</v>
       </c>
@@ -3165,7 +3255,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>64</v>
       </c>
@@ -3182,7 +3272,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>65</v>
       </c>
@@ -3199,7 +3289,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
@@ -3216,7 +3306,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>64</v>
       </c>
@@ -3233,7 +3323,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="70" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
@@ -3250,7 +3340,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="70" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>2.9</v>
       </c>
@@ -3267,7 +3357,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>2.9</v>
       </c>
@@ -3284,7 +3374,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>94</v>
       </c>
@@ -3301,7 +3391,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>94</v>
       </c>
@@ -3318,7 +3408,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>3.1</v>
       </c>
@@ -3335,7 +3425,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>3.1</v>
       </c>
@@ -3352,7 +3442,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>3.2</v>
       </c>
@@ -3369,7 +3459,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="56" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>3.2</v>
       </c>
@@ -3386,7 +3476,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>3.7</v>
       </c>
@@ -3403,7 +3493,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>3.7</v>
       </c>
@@ -3430,24 +3520,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455D7903-7A4F-470E-9AAA-81D792099198}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView rightToLeft="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.4140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="18.75" style="11" customWidth="1"/>
-    <col min="3" max="3" width="37.75" style="11" customWidth="1"/>
-    <col min="4" max="4" width="29.75" style="11" customWidth="1"/>
-    <col min="5" max="5" width="25.75" style="12" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="37.77734375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" style="12" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="27.4140625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="30.08203125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
@@ -3500,7 +3590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>4.0999999999999996</v>
       </c>
@@ -3526,7 +3616,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>229</v>
       </c>
@@ -3552,7 +3642,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>230</v>
       </c>
@@ -3578,7 +3668,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4.3</v>
       </c>
@@ -3604,67 +3694,67 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
         <v>4.5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="84" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+    <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="84" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>4.7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>174</v>
@@ -3673,50 +3763,50 @@
         <v>175</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>4.7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="56" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="56" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>141</v>
@@ -3728,61 +3818,87 @@
         <v>116</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
-        <v>5.0999999999999996</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>192</v>
+        <v>141</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>116</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="98" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>116</v>
       </c>
       <c r="G14" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>6.4</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3804,13 +3920,13 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.08203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="38.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="40.9140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="40.88671875" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3843,7 +3959,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>4.0999999999999996</v>
       </c>
@@ -3864,8 +3980,8 @@
       <c r="A4" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="1" t="s">
         <v>327</v>
       </c>
@@ -3873,12 +3989,12 @@
         <v>328</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="1" t="s">
         <v>329</v>
       </c>
@@ -3886,12 +4002,12 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="1" t="s">
         <v>331</v>
       </c>
@@ -3899,11 +4015,11 @@
         <v>332</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="25" t="s">
         <v>333</v>
       </c>
@@ -3914,12 +4030,12 @@
         <v>335</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="1" t="s">
         <v>336</v>
       </c>
@@ -3944,12 +4060,12 @@
         <v>340</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="1" t="s">
         <v>341</v>
       </c>
@@ -3957,11 +4073,11 @@
         <v>342</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="25" t="s">
         <v>343</v>
       </c>
@@ -3972,12 +4088,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="1" t="s">
         <v>346</v>
       </c>
@@ -4002,12 +4118,12 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="1" t="s">
         <v>341</v>
       </c>
@@ -4015,11 +4131,11 @@
         <v>342</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B15" s="26"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="25" t="s">
         <v>350</v>
       </c>
@@ -4030,12 +4146,12 @@
         <v>345</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="1" t="s">
         <v>352</v>
       </c>
@@ -4060,12 +4176,12 @@
         <v>355</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>4.3</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="1" t="s">
         <v>356</v>
       </c>
@@ -4094,8 +4210,8 @@
       <c r="A20" s="7">
         <v>4.5</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="1" t="s">
         <v>360</v>
       </c>
@@ -4107,8 +4223,8 @@
       <c r="A21" s="7">
         <v>4.5</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="1" t="s">
         <v>361</v>
       </c>
@@ -4120,8 +4236,8 @@
       <c r="A22" s="7">
         <v>4.5</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="1" t="s">
         <v>362</v>
       </c>
@@ -4133,8 +4249,8 @@
       <c r="A23" s="7">
         <v>4.5</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="1" t="s">
         <v>364</v>
       </c>
@@ -4142,7 +4258,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>4.5999999999999996</v>
       </c>
@@ -4159,12 +4275,12 @@
         <v>368</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="1" t="s">
         <v>369</v>
       </c>
@@ -4172,12 +4288,12 @@
         <v>370</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="1" t="s">
         <v>371</v>
       </c>
@@ -4185,12 +4301,12 @@
         <v>372</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="42" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="1" t="s">
         <v>373</v>
       </c>
@@ -4198,7 +4314,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>4.7</v>
       </c>
@@ -4215,12 +4331,12 @@
         <v>377</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>4.7</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="1" t="s">
         <v>378</v>
       </c>
@@ -4228,7 +4344,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>4.9000000000000004</v>
       </c>
@@ -4249,8 +4365,8 @@
       <c r="A31" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="1" t="s">
         <v>382</v>
       </c>
@@ -4258,7 +4374,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>4.1100000000000003</v>
       </c>
@@ -4279,8 +4395,8 @@
       <c r="A33" s="7">
         <v>4.1100000000000003</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="1" t="s">
         <v>382</v>
       </c>
@@ -4288,7 +4404,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>6.4</v>
       </c>
@@ -4309,8 +4425,8 @@
       <c r="A35" s="7">
         <v>6.4</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="1" t="s">
         <v>388</v>
       </c>
@@ -4318,11 +4434,11 @@
         <v>389</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>6.4</v>
       </c>
-      <c r="B36" s="26"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="25" t="s">
         <v>390</v>
       </c>
@@ -4337,8 +4453,8 @@
       <c r="A37" s="7">
         <v>6.4</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="1" t="s">
         <v>393</v>
       </c>
@@ -4346,11 +4462,11 @@
         <v>389</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>6.4</v>
       </c>
-      <c r="B38" s="26"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="25" t="s">
         <v>394</v>
       </c>
@@ -4365,8 +4481,8 @@
       <c r="A39" s="7">
         <v>6.4</v>
       </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="1" t="s">
         <v>397</v>
       </c>
@@ -4378,8 +4494,8 @@
       <c r="A40" s="7">
         <v>6.4</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
       <c r="D40" s="1" t="s">
         <v>398</v>
       </c>
@@ -4389,18 +4505,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="C19:C23"/>
     <mergeCell ref="A1:H1"/>
@@ -4415,6 +4519,18 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4422,22 +4538,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071701CE-A324-4452-B698-F2E194D1AE4B}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="71" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.4140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.4140625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="36.25" style="5" customWidth="1"/>
-    <col min="4" max="4" width="29.75" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.75" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" style="5" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="27.4140625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="30.08203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" style="16" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
@@ -4490,7 +4606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="112" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>7</v>
       </c>
@@ -4516,7 +4632,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>8</v>
       </c>
@@ -4542,7 +4658,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>231</v>
       </c>
@@ -4568,7 +4684,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="56" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>232</v>
       </c>
@@ -4592,6 +4708,84 @@
       </c>
       <c r="H7" s="14" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -4609,15 +4803,15 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.4140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.75" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.4140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="36.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
@@ -4651,7 +4845,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>7</v>
       </c>
@@ -4668,7 +4862,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>7</v>
       </c>
@@ -4685,7 +4879,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>8</v>
       </c>
@@ -4702,7 +4896,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>231</v>
       </c>
@@ -4719,7 +4913,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>231</v>
       </c>
@@ -4736,7 +4930,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>232</v>
       </c>

</xml_diff>

<commit_message>
added use cases for new requirements
</commit_message>
<xml_diff>
--- a/Docs/Use Cases and Acceptance Tests.xlsx
+++ b/Docs/Use Cases and Acceptance Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lidor\BGU 2021 Semester B\סדנה\version 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lidor\BGU 2021 Semester B\סדנה\version 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58D242D5-5961-4F70-B02C-5DB76B5500FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D494988-EDCD-4DD5-A873-A5BA8DB0D4AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34635" yWindow="6045" windowWidth="13830" windowHeight="7170" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usecase1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="481">
   <si>
     <t>שם תרחיש השימוש</t>
   </si>
@@ -81,12 +81,6 @@
   </si>
   <si>
     <t>בעת כניסה למערכת המשתמש נכנס כאורח.</t>
-  </si>
-  <si>
-    <t>אתחול המערכת ומינוי מנהל מסחר</t>
-  </si>
-  <si>
-    <t>בעת אתחול המערכת, מתחברים למערכות החיצוניות (מערכת תשלומים ומערכת הובלות) ומינוי מנהל מסחר</t>
   </si>
   <si>
     <t xml:space="preserve">קונה אורח </t>
@@ -1638,6 +1632,131 @@
   </si>
   <si>
     <t>המנוי אינו מחובר למערכת. ההתראה תושהה ותוצג לו כשיתחבר</t>
+  </si>
+  <si>
+    <t>שמירה לאורך זמן</t>
+  </si>
+  <si>
+    <t>חיבור של המערכת ל- DB</t>
+  </si>
+  <si>
+    <t>המערכת תאותחל על פי מצבה האחרון</t>
+  </si>
+  <si>
+    <t>כל נתוני המערכת שנשמרו לפני "הורדת המערכת", אוחזרו</t>
+  </si>
+  <si>
+    <t>בעת העלאת המערכת, המצב האחרון שלה ישוחזר</t>
+  </si>
+  <si>
+    <t xml:space="preserve">המצב העדכני של המערכת נשמר בסוף כל פעולה </t>
+  </si>
+  <si>
+    <t>הפעולה שבוצעה נשמרה במערכת</t>
+  </si>
+  <si>
+    <t>משתמש מבצע פעולה. הפעולה נשמרת במערכת</t>
+  </si>
+  <si>
+    <t>במקרה של תקלה בחיבור ל- DB, הפעולה תכשל והודעת שגיאה תוצג למשתמש</t>
+  </si>
+  <si>
+    <t>במקרה של תקלה בחיבור ל- DB, המערכת לא תעלה ושגיאה תכתב ב- error log</t>
+  </si>
+  <si>
+    <t>בעת אתחול ראשוני של המערכת, מתחברים למערכות החיצוניות (מערכת תשלומים ומערכת הובלות) ומתבצע מינוי מנהל מסחר</t>
+  </si>
+  <si>
+    <t>אתחול ראשוני של המערכת ומינוי מנהל מסחר</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>אתחול לפי קובץ קונפיגורציה</t>
+  </si>
+  <si>
+    <t>אתחול לא ראשוני של המערכת יתבצע ע"פ קובץ קונפיגורציה שמגדיר את הפרמטרים לאתחול</t>
+  </si>
+  <si>
+    <t>למע' בוצע אתחול ראשוני בעבר. קיים קובץ קונפיגורציה</t>
+  </si>
+  <si>
+    <t>המערכת אותחלה ע"פ קובץ הקונפיגורציה</t>
+  </si>
+  <si>
+    <t>עם אתחול לא ראשוני של המערכת, היא תאותחל לפי קובץ קונפיגורציה</t>
+  </si>
+  <si>
+    <t>במקרה של שגיאה באתחול בחיבור ל- DB/מע' חיצוניות שמוגדר בקובץ בקונפיגורציה, המע' לא תעלה ותכתב שגיאה מתאימה ב- log</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>אתחול לפי "קובץ מצב" (state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">המערכת מאפשרת אתחול במצב שמוגדר ב"קובץ מצב" חיצוני, שמכיל הנחיות לסדרה
+של סיפורי שימוש וארגומנטים להפעלתם </t>
+  </si>
+  <si>
+    <t>לאחר האיתחול המערכת נמצאת במצב המוגדר בקובץ</t>
+  </si>
+  <si>
+    <t>בשלב האתחול המערכת תקרא את הקובץ ותפעיל את סיפורי השימוש המתוארים בו</t>
+  </si>
+  <si>
+    <t>2.c</t>
+  </si>
+  <si>
+    <t>הגשת הצעת קניה</t>
+  </si>
+  <si>
+    <t>בסוג קניה זה משתמש רשאי להציע מחיר עבור מוצר. בעלי החנות או מנהלי החנות בעלי ההרשאה המתאימה רשאים לקבל את הצעת המשתמש, לדחות את הצעת המשמש או להציע הצעת נגד. בסוג קניה זה, משתמש יכול לקנות מוצר רק לאחר קבלת אישור מבעלי/מנהלי החנות</t>
+  </si>
+  <si>
+    <t>המנוי מחובר למערכת. המוצר קיים בחנות</t>
+  </si>
+  <si>
+    <t>המשתמש יקבל אישור/דחיה על הצעתו</t>
+  </si>
+  <si>
+    <t>1. משתמש מציע מחיר עבור מוצר כלשהו בחנות.
+2. בעל החנות או משתמש אחר עם הרשאות מתאימות מקבל את הצעת הקונה.
+3. בעל החנות מאשר את הצעת הקונה.
+4. אישור נשלח לקונה.
+5. הקונה מבצע את הרכישה.</t>
+  </si>
+  <si>
+    <t>3. בעל החנות דוחה את הצעת הקונה. במקרה זה, הקונה יקבל הודעת דחיה ולא יוכל לקנות את המוצר.
+3.א. בעל החנות מציע הצעת נגד לקונה. במקרה זה, הקונה יקבל את הצעת הנגד ויוכל להחליט האם לרכוש או לא</t>
+  </si>
+  <si>
+    <t>צפיה בהכנסה הכוללת של המע' בחתך יומי</t>
+  </si>
+  <si>
+    <t>מנהל המערכת יכול לצפות בהכנסה הכוללת של המערכת בחתך יומי</t>
+  </si>
+  <si>
+    <t>1. מנהל המערכת מבקש לצפות בהכנסה הכולל של המערכת בחתך יומי.
+2. המערכת מציגה את הנתון למנהל המע'</t>
+  </si>
+  <si>
+    <t>2.d.i</t>
+  </si>
+  <si>
+    <t>2.d.ii</t>
+  </si>
+  <si>
+    <t>צפיה בהכנסה הכוללת של חנות בחתך יומי</t>
+  </si>
+  <si>
+    <t>בעלי חנות יכולים לצפות בהכנסה הכוללת של חנותם בחתך יומי</t>
+  </si>
+  <si>
+    <t>1. בעל החנות מבקש לצפות בהכנסה הכולל של החנות בחתך יומי.
+2. המערכת מציגה את הנתון לבעל החנות</t>
   </si>
 </sst>
 </file>
@@ -1795,7 +1914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1857,6 +1976,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1872,11 +1994,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2158,10 +2283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A21" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView rightToLeft="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2172,34 +2297,34 @@
     <col min="4" max="4" width="29.77734375" style="5" customWidth="1"/>
     <col min="5" max="5" width="19.77734375" style="5" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="40.5546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="40.5546875" style="11" customWidth="1"/>
     <col min="8" max="8" width="42.77734375" style="5" customWidth="1"/>
     <col min="9" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -2220,7 +2345,7 @@
       <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -2232,545 +2357,621 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="E9" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>2.1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="6" t="s">
+    </row>
+    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="G11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>2.6</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="H13" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>2.7</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H15" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H16" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="F17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="G20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>2.9</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="F24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H21" s="2" t="s">
+    </row>
+    <row r="26" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
-        <v>3.7</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="E26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="G26" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="H26" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>113</v>
+    </row>
+    <row r="27" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -2788,7 +2989,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2802,32 +3003,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="A1" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2835,16 +3036,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2852,16 +3053,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2869,16 +3070,16 @@
         <v>2.1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2886,16 +3087,16 @@
         <v>2.1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2903,16 +3104,16 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2920,16 +3121,16 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2937,16 +3138,16 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2954,16 +3155,16 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2971,16 +3172,16 @@
         <v>2.4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2988,16 +3189,16 @@
         <v>2.4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -3005,16 +3206,16 @@
         <v>2.5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -3022,50 +3223,50 @@
         <v>2.5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -3073,16 +3274,16 @@
         <v>2.6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -3090,16 +3291,16 @@
         <v>2.6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -3107,16 +3308,16 @@
         <v>2.6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -3124,16 +3325,16 @@
         <v>2.6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -3141,16 +3342,16 @@
         <v>2.7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -3158,186 +3359,186 @@
         <v>2.7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="72" x14ac:dyDescent="0.3">
@@ -3345,16 +3546,16 @@
         <v>2.9</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -3362,50 +3563,50 @@
         <v>2.9</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -3413,16 +3614,16 @@
         <v>3.1</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -3430,16 +3631,16 @@
         <v>3.1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -3447,16 +3648,16 @@
         <v>3.2</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -3464,16 +3665,16 @@
         <v>3.2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -3481,16 +3682,16 @@
         <v>3.7</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -3498,16 +3699,16 @@
         <v>3.7</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -3520,12 +3721,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455D7903-7A4F-470E-9AAA-81D792099198}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3541,28 +3742,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -3595,77 +3796,77 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="E4" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="F5" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="F6" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -3673,25 +3874,25 @@
         <v>4.3</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -3699,25 +3900,25 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="H8" s="9" t="s">
         <v>420</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>421</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -3725,25 +3926,25 @@
         <v>4.5</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="F9" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -3751,25 +3952,25 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>176</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -3777,25 +3978,25 @@
         <v>4.7</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="G11" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -3803,25 +4004,25 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>186</v>
-      </c>
       <c r="H12" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -3829,25 +4030,25 @@
         <v>4.1100000000000003</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>189</v>
-      </c>
       <c r="H13" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -3855,25 +4056,25 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -3881,25 +4082,77 @@
         <v>6.4</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>200</v>
-      </c>
       <c r="H15" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3931,49 +4184,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="A1" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>235</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -3983,10 +4236,10 @@
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -3996,10 +4249,10 @@
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4007,12 +4260,12 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B6" s="27"/>
-      <c r="C6" s="26"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4020,190 +4273,190 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B7" s="27"/>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B10" s="27"/>
-      <c r="C10" s="26"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B11" s="27"/>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+        <v>227</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>348</v>
+        <v>228</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>346</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B14" s="27"/>
-      <c r="C14" s="26"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B15" s="27"/>
-      <c r="C15" s="25" t="s">
-        <v>350</v>
+      <c r="C15" s="26" t="s">
+        <v>348</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
+        <v>228</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>4.3</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>158</v>
+      <c r="B17" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>156</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>4.3</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>4.5</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>165</v>
+      <c r="B19" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>163</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -4213,10 +4466,10 @@
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
       <c r="D20" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -4226,10 +4479,10 @@
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
       <c r="D21" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -4239,40 +4492,40 @@
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
       <c r="D22" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>4.5</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B24" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C24" s="25" t="s">
+      <c r="B24" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -4282,10 +4535,10 @@
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
       <c r="D25" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -4295,130 +4548,130 @@
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
       <c r="D26" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>4.7</v>
       </c>
-      <c r="B28" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="C28" s="25" t="s">
+      <c r="B28" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>4.7</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B30" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>184</v>
+      <c r="B30" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>182</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>4.1100000000000003</v>
       </c>
-      <c r="B32" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>384</v>
+      <c r="B32" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>382</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>4.1100000000000003</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>6.4</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="C34" s="25" t="s">
+      <c r="B34" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -4426,12 +4679,12 @@
         <v>6.4</v>
       </c>
       <c r="B35" s="27"/>
-      <c r="C35" s="26"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -4439,14 +4692,14 @@
         <v>6.4</v>
       </c>
       <c r="B36" s="27"/>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="26" t="s">
+        <v>388</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -4454,12 +4707,12 @@
         <v>6.4</v>
       </c>
       <c r="B37" s="27"/>
-      <c r="C37" s="26"/>
+      <c r="C37" s="28"/>
       <c r="D37" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4467,14 +4720,14 @@
         <v>6.4</v>
       </c>
       <c r="B38" s="27"/>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -4484,27 +4737,39 @@
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
       <c r="D39" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>6.4</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
       <c r="D40" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="C19:C23"/>
     <mergeCell ref="A1:H1"/>
@@ -4519,18 +4784,6 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4538,10 +4791,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071701CE-A324-4452-B698-F2E194D1AE4B}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView rightToLeft="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4552,33 +4805,33 @@
     <col min="4" max="4" width="29.77734375" style="5" customWidth="1"/>
     <col min="5" max="5" width="19.77734375" style="5" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" style="16" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="30.109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
@@ -4599,10 +4852,10 @@
       <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4611,25 +4864,25 @@
         <v>7</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="E4" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="F4" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="G4" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="H4" s="29" t="s">
         <v>207</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -4637,155 +4890,207 @@
         <v>8</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>116</v>
+      <c r="H5" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B6" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>116</v>
+      <c r="H6" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>116</v>
+      <c r="H7" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>427</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>428</v>
-      </c>
       <c r="D9" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>433</v>
+      <c r="H9" s="2" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="G10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>6.1</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>442</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>443</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>6.2</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -4817,32 +5122,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="A1" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>235</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4850,16 +5155,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4867,16 +5172,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -4884,67 +5189,67 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>